<commit_message>
Changes in Requirements HU
</commit_message>
<xml_diff>
--- a/02-Requirements/Work matrix HU.xlsx
+++ b/02-Requirements/Work matrix HU.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNIVERSIDAD\SEXTO SEMESTRE\DESARROLLO WEB\Actividad 5 GIT\DevelopersTeam2FashionStore\02-Requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Documents\Trabajos de Git Hub\DevelopersTeam2FashionStore\02-Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD7346D-8A88-40BC-AE71-F0AA221CB8F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC27B8D-102C-45B3-B762-EBB2DE9CB0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{5153D9AA-365A-42B5-8A27-3DE9F46FB439}"/>
+    <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11111" xr2:uid="{5153D9AA-365A-42B5-8A27-3DE9F46FB439}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="97">
   <si>
     <t>Matriz de Marco de Trabajo de HU</t>
   </si>
@@ -114,9 +106,6 @@
     <t>Conocer datos del proveedor</t>
   </si>
   <si>
-    <t>Saber los tipos de proveedores que tengo</t>
-  </si>
-  <si>
     <t>GR 02</t>
   </si>
   <si>
@@ -144,9 +133,6 @@
     <t>Registro de salidad de productos</t>
   </si>
   <si>
-    <t>El sistema debe pedir los datos del proveedor como: Nombre, cédula, dirección y teléfono.</t>
-  </si>
-  <si>
     <t>Ingreso de los productos de forma exitosa.</t>
   </si>
   <si>
@@ -259,6 +245,81 @@
   </si>
   <si>
     <t>Lista de productos vendidos</t>
+  </si>
+  <si>
+    <t>REQ006</t>
+  </si>
+  <si>
+    <t>Llevar un control de los proveedores</t>
+  </si>
+  <si>
+    <t>REQ008</t>
+  </si>
+  <si>
+    <t>REQ007</t>
+  </si>
+  <si>
+    <t>Listar Proveedor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Listar Proveedor</t>
+  </si>
+  <si>
+    <t>Conocer los proveedores que registro</t>
+  </si>
+  <si>
+    <t>Listar los proveedores registrados</t>
+  </si>
+  <si>
+    <t>El sistema debe pedir los datos del proveedor como: ID, Nombre, Dirección, Teléfono, Tipo de producto y Total.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe listar los datos del proveedor: Nombre, Dirección, Teléfono, Tipo de Producto.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Modificar Proveedor</t>
+  </si>
+  <si>
+    <t>Cambiar datos de proveedor</t>
+  </si>
+  <si>
+    <t>Actualizar datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema contara con botones de Editar, Eliminar y Agregar </t>
+  </si>
+  <si>
+    <t>Modificacion de datos de forma exitosa</t>
+  </si>
+  <si>
+    <t>El usuario podra modificar los datos a su gusto</t>
+  </si>
+  <si>
+    <t>Modificar Proveedor</t>
+  </si>
+  <si>
+    <t>REQ009</t>
+  </si>
+  <si>
+    <t>Menu Proveedor</t>
+  </si>
+  <si>
+    <t>Menú Proveedor</t>
+  </si>
+  <si>
+    <t>Opciones a realizar con el Proveedor</t>
+  </si>
+  <si>
+    <t>Eleguir opciones a realizar con el proveedor</t>
+  </si>
+  <si>
+    <t>El sistema contara con un menu en el que se indique la opcion proveedores y poder eleguir alguna acción</t>
+  </si>
+  <si>
+    <t>Mostrar opciones y direccionar a la accion de la opcion</t>
+  </si>
+  <si>
+    <t>El usuario podra eleguir 2 opciones</t>
   </si>
 </sst>
 </file>
@@ -690,28 +751,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4527FA18-ABB7-4CFC-8EEF-33C17DFFDA53}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.77734375" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" customWidth="1"/>
-    <col min="6" max="6" width="18.21875" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1"/>
-    <col min="8" max="8" width="13.77734375" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" customWidth="1"/>
-    <col min="12" max="12" width="19.6640625" customWidth="1"/>
-    <col min="13" max="13" width="16.44140625" customWidth="1"/>
-    <col min="14" max="14" width="11.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.796875" customWidth="1"/>
+    <col min="3" max="3" width="14.59765625" customWidth="1"/>
+    <col min="4" max="4" width="14.3984375" customWidth="1"/>
+    <col min="5" max="5" width="15.796875" customWidth="1"/>
+    <col min="6" max="6" width="18.19921875" customWidth="1"/>
+    <col min="7" max="7" width="17.296875" customWidth="1"/>
+    <col min="8" max="8" width="13.796875" customWidth="1"/>
+    <col min="9" max="9" width="13.09765625" customWidth="1"/>
+    <col min="12" max="12" width="19.69921875" customWidth="1"/>
+    <col min="13" max="13" width="16.3984375" customWidth="1"/>
+    <col min="14" max="14" width="11.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="20.95" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -729,7 +790,7 @@
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
     </row>
-    <row r="2" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="55.9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -773,30 +834,30 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="91.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="92.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I3" s="2">
         <v>44928</v>
@@ -808,39 +869,39 @@
         <v>18</v>
       </c>
       <c r="L3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="M3" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="91.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:14" ht="92.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I4" s="2">
         <v>44929</v>
@@ -852,39 +913,39 @@
         <v>18</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="91.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="92.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I5" s="2">
         <v>44929</v>
@@ -896,39 +957,39 @@
         <v>18</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="91.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="92.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I6" s="2">
         <v>44929</v>
@@ -940,39 +1001,39 @@
         <v>18</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="91.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="92.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I7" s="2">
         <v>44929</v>
@@ -984,18 +1045,18 @@
         <v>18</v>
       </c>
       <c r="L7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="N7" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="M7" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="91.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:14" ht="92.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>23</v>
@@ -1004,22 +1065,22 @@
         <v>24</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="I8" s="2">
-        <v>44888</v>
+        <v>44929</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>17</v>
@@ -1028,42 +1089,86 @@
         <v>18</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="73.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="2">
+        <v>44929</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="M9" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="N9" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="81.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="I10" s="2">
-        <v>44888</v>
+        <v>44929</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>17</v>
@@ -1072,42 +1177,42 @@
         <v>18</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>39</v>
+        <v>86</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="69" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="80.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>22</v>
+        <v>89</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="I11" s="2">
-        <v>44888</v>
+        <v>44929</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>17</v>
@@ -1116,13 +1221,133 @@
         <v>18</v>
       </c>
       <c r="L11" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="55.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+    </row>
+    <row r="13" spans="1:14" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="1:14" ht="94.05" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N11" s="4" t="s">
+      <c r="C14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="2">
+        <v>44888</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="67.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>31</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="2">
+        <v>44888</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1131,11 +1356,11 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K10:K11 K3:K8" xr:uid="{83BC428A-36F9-42CB-941F-6010D337FBCE}">
-      <formula1>$K$25:$K$28</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K3:K15" xr:uid="{83BC428A-36F9-42CB-941F-6010D337FBCE}">
+      <formula1>$K$29:$K$32</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J10:J11 J3:J8" xr:uid="{167A1E12-CD84-4510-AB00-21DA3727B760}">
-      <formula1>$J$25:$J$27</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J3:J15" xr:uid="{167A1E12-CD84-4510-AB00-21DA3727B760}">
+      <formula1>$J$29:$J$31</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>